<commit_message>
update code bai 28: đọc data test từ file excel
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/dataCRM.xlsx
+++ b/src/test/resources/testdata/dataCRM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SeleniumMavenTestNGParallel\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD652A3-361C-4BD8-8A37-B61A5CFF9D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D405CBAB-A8BC-4E6E-8E04-B8C905601006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="21600" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>EMAIL</t>
   </si>
@@ -41,6 +41,33 @@
   </si>
   <si>
     <t>namtest@gmail.com</t>
+  </si>
+  <si>
+    <t>CUSTOMER_NAME</t>
+  </si>
+  <si>
+    <t>hatest_290925</t>
+  </si>
+  <si>
+    <t>PHONE</t>
+  </si>
+  <si>
+    <t>WEBSITE</t>
+  </si>
+  <si>
+    <t>0965897785</t>
+  </si>
+  <si>
+    <t>hatest.com.vn</t>
+  </si>
+  <si>
+    <t>TEST_RESULT</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -65,12 +92,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill/>
@@ -89,16 +119,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -382,44 +416,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="25.5546875"/>
     <col min="2" max="2" customWidth="true" width="24.44140625"/>
+    <col min="3" max="3" customWidth="true" width="13.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
       <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
+      <c r="C1" t="s" s="0">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="0">
         <v>123</v>
       </c>
+      <c r="C2" t="s" s="5">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="0">
         <v>456</v>
       </c>
+      <c r="C3" t="s" s="6">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s" s="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -435,12 +479,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F957D2-3B4F-47C4-9214-D3EC00533BE8}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="22.44140625"/>
+    <col min="2" max="2" customWidth="true" width="26.5546875"/>
+    <col min="3" max="3" customWidth="true" width="20.33203125"/>
+    <col min="4" max="4" customWidth="true" width="15.88671875"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{3CC3A571-F39B-45D7-97D1-E615CA37B655}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
code bài 30: demo Take Screenshot phan 1
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/dataCRM.xlsx
+++ b/src/test/resources/testdata/dataCRM.xlsx
@@ -3,22 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SeleniumMavenTestNGParallel\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D405CBAB-A8BC-4E6E-8E04-B8C905601006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CE65A3-0E0C-4416-8997-F51066490865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="21600" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Customer" sheetId="2" r:id="rId2"/>
+    <sheet name="Login_DataProvider" sheetId="3" r:id="rId2"/>
+    <sheet name="Customer" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>EMAIL</t>
   </si>
@@ -40,9 +41,6 @@
     <t>phuongtest@gmail.com</t>
   </si>
   <si>
-    <t>namtest@gmail.com</t>
-  </si>
-  <si>
     <t>CUSTOMER_NAME</t>
   </si>
   <si>
@@ -68,13 +66,15 @@
   </si>
   <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>admin@example.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -92,7 +92,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,9 +101,6 @@
     </fill>
     <fill>
       <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill/>
     </fill>
   </fills>
   <borders count="1">
@@ -119,20 +116,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -418,36 +406,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.5546875"/>
-    <col min="2" max="2" customWidth="true" width="24.44140625"/>
-    <col min="3" max="3" customWidth="true" width="13.33203125"/>
+    <col min="1" max="1" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
-        <v>11</v>
+      <c r="C1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2">
         <v>123</v>
       </c>
-      <c r="C2" t="s" s="5">
+      <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -455,29 +443,93 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <v>456</v>
       </c>
-      <c r="C3" t="s" s="6">
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
+      <c r="B4">
+        <v>123456</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{19359BE9-F963-4574-9311-0EA583DEB751}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{9997E4EA-856A-4494-9342-42EA189CCC5E}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{0C23D041-E07B-4284-87A1-99F39A3CAD0B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2917AC9-D6DA-4288-B494-6BA05910363A}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>123456</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{CD53FFCB-A66D-4CA2-B161-1698A4D10399}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{26E72818-3586-49F6-8DCF-AC762D13025F}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{E4A60847-4120-4146-9F73-C758E563153C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F957D2-3B4F-47C4-9214-D3EC00533BE8}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -487,38 +539,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.44140625"/>
-    <col min="2" max="2" customWidth="true" width="26.5546875"/>
-    <col min="3" max="3" customWidth="true" width="20.33203125"/>
-    <col min="4" max="4" customWidth="true" width="15.88671875"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s" s="0">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
-        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update code in lesson 29: Use DataProvider in TestNG to pass test data.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/dataCRM.xlsx
+++ b/src/test/resources/testdata/dataCRM.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SeleniumMavenTestNGParallel\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CE65A3-0E0C-4416-8997-F51066490865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -74,7 +73,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -403,21 +402,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,7 +427,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -439,7 +438,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -450,7 +449,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -463,9 +462,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{19359BE9-F963-4574-9311-0EA583DEB751}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{9997E4EA-856A-4494-9342-42EA189CCC5E}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{0C23D041-E07B-4284-87A1-99F39A3CAD0B}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -473,20 +472,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2917AC9-D6DA-4288-B494-6BA05910363A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -502,7 +501,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -510,7 +509,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -520,9 +519,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{CD53FFCB-A66D-4CA2-B161-1698A4D10399}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{26E72818-3586-49F6-8DCF-AC762D13025F}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{E4A60847-4120-4146-9F73-C758E563153C}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -530,22 +529,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F957D2-3B4F-47C4-9214-D3EC00533BE8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="2" width="26.5546875" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -559,7 +558,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -575,7 +574,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{3CC3A571-F39B-45D7-97D1-E615CA37B655}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>